<commit_message>
The Project was done You'd better check it out İf there is somethingwron please feedback me ciao
</commit_message>
<xml_diff>
--- a/src/test/java/Resources/LCWtestCases.xlsx
+++ b/src/test/java/Resources/LCWtestCases.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\java_kursu\Javakursu3\LCWwebsiteTesting\src\test\java\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\IdeaProjects\LCWwebsiteTesting\src\test\java\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DB8800-6AAB-40D8-9D9F-795A0A918FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="70">
   <si>
     <t>TestID</t>
   </si>
@@ -196,13 +197,72 @@
   </si>
   <si>
     <t>kendi nameniz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orcun ILGEN </t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>User checks the live-chat out whether works properly</t>
+  </si>
+  <si>
+    <t>1. Open website / go to mainpage in datatable scenario with background</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>|clickincokie1 | / click in the cokie in order to disappear it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">| clickninanladım| click in the close tab in order to end it up </t>
+  </si>
+  <si>
+    <t>|livesupportclick | click in the live-chat to make sure checking it out</t>
+  </si>
+  <si>
+    <t>|clickinorders | click in the "orders" to see info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">| quitlick| click in the close tab in ordert to exit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">| quitclickYes | click in the "are sure to exit" button in order to end it up completely </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESULT BİNGOOOOOOOOOOOOOOOOOO!!!!! :))    |^_^| </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+        <charset val="162"/>
+      </rPr>
+      <t>AND</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Click on the element in the dialog</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,6 +329,20 @@
       <family val="2"/>
       <charset val="162"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Bahnschrift SemiBold"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -297,7 +371,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -319,6 +393,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Köprü" xfId="1" builtinId="8"/>
@@ -357,7 +432,7 @@
         <xdr:cNvPr id="3" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7407CC7C-C202-4CFC-AD5C-8A8407F105C3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -404,7 +479,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Resim 3"/>
+        <xdr:cNvPr id="4" name="Resim 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -692,11 +773,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I155"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="B55" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,6 +1112,63 @@
         <v>19</v>
       </c>
     </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>58</v>
+      </c>
+      <c r="C59" t="s">
+        <v>59</v>
+      </c>
+      <c r="E59" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="E60" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E61" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>61</v>
+      </c>
+      <c r="E62" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E64" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E66" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E67" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
     <row r="84" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
@@ -1117,20 +1255,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="F2" r:id="rId2"/>
-    <hyperlink ref="F30" r:id="rId3"/>
-    <hyperlink ref="D58" r:id="rId4"/>
-    <hyperlink ref="D85" r:id="rId5"/>
-    <hyperlink ref="D120" r:id="rId6"/>
-    <hyperlink ref="D155" r:id="rId7"/>
-    <hyperlink ref="D30" r:id="rId8"/>
-    <hyperlink ref="F58" r:id="rId9"/>
-    <hyperlink ref="F85" r:id="rId10"/>
-    <hyperlink ref="F120" r:id="rId11"/>
-    <hyperlink ref="F155" r:id="rId12"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F30" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D58" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D85" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D120" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D155" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D30" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F58" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F85" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="F120" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F155" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <drawing r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Muharrem - TestCase added.
</commit_message>
<xml_diff>
--- a/src/test/java/Resources/LCWtestCases.xlsx
+++ b/src/test/java/Resources/LCWtestCases.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkara\IdeaProjects\LCWwebsiteTesting\src\test\java\Resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7668"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="103">
   <si>
     <t>TestID</t>
   </si>
@@ -254,13 +259,88 @@
   </si>
   <si>
     <t>AND Click on the a random product</t>
+  </si>
+  <si>
+    <t>The user should be able to select any of the Blouses from the SHADE WOMEN'S PRODUCTS category and go to the payment page. They should be able to see if there is a discount.</t>
+  </si>
+  <si>
+    <t>2. Verify that you are on the home page</t>
+  </si>
+  <si>
+    <t>3. Click on "SHADE KADIN ÜRÜNLERİ" title opportunity</t>
+  </si>
+  <si>
+    <t>4. Filter products by "Bluz" and choose a random product</t>
+  </si>
+  <si>
+    <t>5. If available, choose random size and color and add to cart</t>
+  </si>
+  <si>
+    <t>6. Click on the addToCart</t>
+  </si>
+  <si>
+    <t>7. Click on the Cart</t>
+  </si>
+  <si>
+    <t>8. Product price and discount rate</t>
+  </si>
+  <si>
+    <t>9. Click on the Payment</t>
+  </si>
+  <si>
+    <t>10. Fill out the form on the payment page</t>
+  </si>
+  <si>
+    <t>11. Click on the save button</t>
+  </si>
+  <si>
+    <t>And Click on MARKALARA ÖZEL title from the main page</t>
+  </si>
+  <si>
+    <t>And Click on SHADE KADIN ÜRÜNLERİ title opportunity</t>
+  </si>
+  <si>
+    <t>And Filter products by Bluz and choose a random product</t>
+  </si>
+  <si>
+    <t>And If available, choose random size and color and add to cart</t>
+  </si>
+  <si>
+    <t>And Click on the addToCart</t>
+  </si>
+  <si>
+    <t>And Click on the Cart</t>
+  </si>
+  <si>
+    <t>And Product price and discount rate</t>
+  </si>
+  <si>
+    <t>And Click on the Payment</t>
+  </si>
+  <si>
+    <t>And Fill out the form on the payment page</t>
+  </si>
+  <si>
+    <t>Then Click on the save button</t>
+  </si>
+  <si>
+    <t>LCW home page should be open /display</t>
+  </si>
+  <si>
+    <t>User should be able to click on "SHADE KADIN ÜRÜNLERİ" title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should be able to choose "Bluz" filter </t>
+  </si>
+  <si>
+    <t>User should be able if available choose random size and color and add to cart</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,6 +407,15 @@
       <family val="2"/>
       <charset val="162"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -355,7 +444,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -380,6 +469,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Köprü" xfId="1" builtinId="8"/>
@@ -418,7 +508,7 @@
         <xdr:cNvPr id="3" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7407CC7C-C202-4CFC-AD5C-8A8407F105C3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7407CC7C-C202-4CFC-AD5C-8A8407F105C3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -430,7 +520,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -746,34 +836,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I155"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView tabSelected="1" topLeftCell="A131" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="J155" sqref="J155"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" customWidth="1"/>
-    <col min="5" max="5" width="65.7109375" customWidth="1"/>
-    <col min="6" max="6" width="33.42578125" customWidth="1"/>
-    <col min="7" max="7" width="83.42578125" customWidth="1"/>
-    <col min="8" max="8" width="26.140625" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" customWidth="1"/>
+    <col min="4" max="4" width="34.109375" customWidth="1"/>
+    <col min="5" max="5" width="65.6640625" customWidth="1"/>
+    <col min="6" max="6" width="33.44140625" customWidth="1"/>
+    <col min="7" max="7" width="83.44140625" customWidth="1"/>
+    <col min="8" max="8" width="26.109375" customWidth="1"/>
+    <col min="9" max="9" width="22.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1">
+    <row r="1" spans="1:9" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -802,7 +892,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30.75" customHeight="1">
+    <row r="2" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -831,7 +921,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="20.25" customHeight="1">
+    <row r="3" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E3" s="2" t="s">
         <v>21</v>
       </c>
@@ -843,7 +933,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="33" customHeight="1">
+    <row r="4" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E4" s="8" t="s">
         <v>22</v>
       </c>
@@ -855,7 +945,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75">
+    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E5" s="8" t="s">
         <v>26</v>
       </c>
@@ -866,7 +956,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75">
+    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E6" s="2" t="s">
         <v>25</v>
       </c>
@@ -877,7 +967,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75">
+    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E7" s="2" t="s">
         <v>23</v>
       </c>
@@ -888,7 +978,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75">
+    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E8" s="2" t="s">
         <v>24</v>
       </c>
@@ -899,7 +989,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75">
+    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E9" s="2" t="s">
         <v>27</v>
       </c>
@@ -910,7 +1000,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75">
+    <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E10" s="2" t="s">
         <v>28</v>
       </c>
@@ -921,7 +1011,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75">
+    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E11" s="2" t="s">
         <v>29</v>
       </c>
@@ -932,7 +1022,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75">
+    <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E12" s="2" t="s">
         <v>30</v>
       </c>
@@ -943,82 +1033,82 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75">
+    <row r="13" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75">
+    <row r="14" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E14" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75">
+    <row r="15" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E15" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75">
+    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E16" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75">
+    <row r="17" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E17" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="30.75" customHeight="1">
+    <row r="18" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E18" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.75">
+    <row r="19" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E19" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75">
+    <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E20" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75">
+    <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E21" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75">
+    <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E22" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75">
+    <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E23" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75">
+    <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E24" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75">
+    <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E25" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.75">
+    <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E26" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15.75">
+    <row r="27" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E27" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="5" customFormat="1">
+    <row r="29" spans="1:9" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1029,7 +1119,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="4"/>
     </row>
-    <row r="30" spans="1:9" ht="15.75">
+    <row r="30" spans="1:9" ht="45.6" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>51</v>
       </c>
@@ -1055,7 +1145,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15.75">
+    <row r="31" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E31" s="2" t="s">
         <v>21</v>
       </c>
@@ -1067,7 +1157,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.75">
+    <row r="32" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E32" s="2" t="s">
         <v>59</v>
       </c>
@@ -1079,7 +1169,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="5:8" ht="15.75">
+    <row r="33" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E33" s="2" t="s">
         <v>61</v>
       </c>
@@ -1090,7 +1180,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="5:8" ht="15.75">
+    <row r="34" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E34" s="2" t="s">
         <v>63</v>
       </c>
@@ -1101,7 +1191,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="5:8" ht="15.75">
+    <row r="35" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E35" s="2" t="s">
         <v>65</v>
       </c>
@@ -1112,7 +1202,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="5:8" ht="15.75">
+    <row r="36" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E36" s="2" t="s">
         <v>67</v>
       </c>
@@ -1123,7 +1213,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="5:8" ht="15.75">
+    <row r="37" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E37" s="2" t="s">
         <v>68</v>
       </c>
@@ -1134,7 +1224,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="5:8" ht="15.75">
+    <row r="38" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E38" s="2" t="s">
         <v>69</v>
       </c>
@@ -1145,7 +1235,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="5:8" ht="15.75">
+    <row r="39" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E39" s="2" t="s">
         <v>70</v>
       </c>
@@ -1156,7 +1246,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="5:8" ht="15.75">
+    <row r="40" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E40" s="2" t="s">
         <v>71</v>
       </c>
@@ -1167,7 +1257,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="5:8" ht="15.75">
+    <row r="41" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E41" s="2" t="s">
         <v>72</v>
       </c>
@@ -1178,7 +1268,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="5:8" ht="15.75">
+    <row r="42" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E42" s="2" t="s">
         <v>73</v>
       </c>
@@ -1189,75 +1279,75 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="5:8" ht="15.75">
+    <row r="43" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E43" s="2"/>
     </row>
-    <row r="44" spans="5:8" ht="15.75">
+    <row r="44" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E44" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="5:8" ht="15.75">
+    <row r="45" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E45" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="5:8" ht="15.75">
+    <row r="46" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E46" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="5:8" ht="15.75">
+    <row r="47" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E47" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="5:8" ht="15.75">
+    <row r="48" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E48" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="15.75">
+    <row r="49" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E49" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="15.75">
+    <row r="50" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E50" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="15.75">
+    <row r="51" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E51" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="15.75">
+    <row r="52" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E52" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="15.75">
+    <row r="53" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E53" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="15.75">
+    <row r="54" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E54" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="15.75">
+    <row r="55" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E55" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="15.75">
+    <row r="56" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E56" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="1:9" s="5" customFormat="1">
+    <row r="57" spans="1:9" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -1268,7 +1358,7 @@
       <c r="H57" s="3"/>
       <c r="I57" s="4"/>
     </row>
-    <row r="58" spans="1:9" ht="15.75">
+    <row r="58" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>54</v>
       </c>
@@ -1285,7 +1375,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="84" spans="1:9" s="5" customFormat="1">
+    <row r="84" spans="1:9" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
@@ -1296,7 +1386,7 @@
       <c r="H84" s="3"/>
       <c r="I84" s="4"/>
     </row>
-    <row r="85" spans="1:9" ht="15.75">
+    <row r="85" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>55</v>
       </c>
@@ -1313,7 +1403,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="119" spans="1:9" s="5" customFormat="1">
+    <row r="119" spans="1:9" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" s="3"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
@@ -1324,7 +1414,7 @@
       <c r="H119" s="3"/>
       <c r="I119" s="4"/>
     </row>
-    <row r="120" spans="1:9" ht="15.75">
+    <row r="120" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>56</v>
       </c>
@@ -1341,7 +1431,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="154" spans="1:9" s="5" customFormat="1">
+    <row r="154" spans="1:9" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A154" s="3"/>
       <c r="B154" s="3"/>
       <c r="C154" s="3"/>
@@ -1352,7 +1442,7 @@
       <c r="H154" s="3"/>
       <c r="I154" s="4"/>
     </row>
-    <row r="155" spans="1:9" ht="15.75">
+    <row r="155" spans="1:9" ht="90.6" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>57</v>
       </c>
@@ -1360,13 +1450,205 @@
         <v>16</v>
       </c>
       <c r="C155" s="8" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="D155" s="7" t="s">
         <v>19</v>
       </c>
+      <c r="E155" t="s">
+        <v>20</v>
+      </c>
       <c r="F155" s="7" t="s">
         <v>19</v>
+      </c>
+      <c r="G155" t="s">
+        <v>99</v>
+      </c>
+      <c r="H155" t="s">
+        <v>11</v>
+      </c>
+      <c r="I155" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E156" t="s">
+        <v>79</v>
+      </c>
+      <c r="G156" t="s">
+        <v>42</v>
+      </c>
+      <c r="H156" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E157" t="s">
+        <v>80</v>
+      </c>
+      <c r="G157" t="s">
+        <v>100</v>
+      </c>
+      <c r="H157" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E158" t="s">
+        <v>81</v>
+      </c>
+      <c r="G158" t="s">
+        <v>101</v>
+      </c>
+      <c r="H158" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E159" t="s">
+        <v>82</v>
+      </c>
+      <c r="G159" t="s">
+        <v>102</v>
+      </c>
+      <c r="H159" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E160" t="s">
+        <v>83</v>
+      </c>
+      <c r="G160" t="s">
+        <v>46</v>
+      </c>
+      <c r="H160" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="161" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E161" t="s">
+        <v>84</v>
+      </c>
+      <c r="G161" t="s">
+        <v>47</v>
+      </c>
+      <c r="H161" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="162" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E162" t="s">
+        <v>85</v>
+      </c>
+      <c r="G162" t="s">
+        <v>48</v>
+      </c>
+      <c r="H162" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="163" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E163" t="s">
+        <v>86</v>
+      </c>
+      <c r="G163" t="s">
+        <v>49</v>
+      </c>
+      <c r="H163" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="164" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E164" t="s">
+        <v>87</v>
+      </c>
+      <c r="G164" t="s">
+        <v>50</v>
+      </c>
+      <c r="H164" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="165" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E165" t="s">
+        <v>88</v>
+      </c>
+      <c r="G165" t="s">
+        <v>9</v>
+      </c>
+      <c r="H165" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="167" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E167" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="168" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E168" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="169" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E169" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="170" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E170" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="171" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E171" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="172" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E172" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="173" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E173" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="174" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E174" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="175" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E175" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="176" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E176" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="177" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E177" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="178" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E178" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="179" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E179" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="180" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E180" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>